<commit_message>
Added method for storing generated IDs in excel file, and appeding them
</commit_message>
<xml_diff>
--- a/generated_pallets.xlsx
+++ b/generated_pallets.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing_pallets" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Testing_sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,7 +19,7 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -62,9 +62,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -147,44 +147,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -211,14 +211,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,6 +263,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,166 +292,162 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -425,7 +457,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,350 +493,700 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ID:dbwxos5877, Pallet created:2024-07-22</t>
+          <t>ID:djibcl9275, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ID:zssmnz5581, Pallet created:2024-07-22</t>
+          <t>ID:zpanxm4369, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ID:ygixzx8765, Pallet created:2024-07-22</t>
+          <t>ID:hkxauq5442, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ID:dyfpsw3927, Pallet created:2024-07-22</t>
+          <t>ID:ipqhqt6536, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ID:tilhgm3952, Pallet created:2024-07-22</t>
+          <t>ID:ffdbmq0210, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ID:rkhvpt8413, Pallet created:2024-07-22</t>
+          <t>ID:jjzazu3971, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ID:fzmwjr7077, Pallet created:2024-07-22</t>
+          <t>ID:vyncmy5537, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ID:pzjqdw5617, Pallet created:2024-07-22</t>
+          <t>ID:kjxapu7155, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ID:cvcgaz8918, Pallet created:2024-07-22</t>
+          <t>ID:ifdtua2422, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ID:smmbyy6408, Pallet created:2024-07-22</t>
+          <t>ID:zcoxco3617, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ID:chkqqr7878, Pallet created:2024-07-22</t>
+          <t>ID:ztkqpj6704, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ID:twzxjg1528, Pallet created:2024-07-22</t>
+          <t>ID:yrzzhm9850, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ID:pgwzju5428, Pallet created:2024-07-22</t>
+          <t>ID:dfmxqi9909, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ID:oinejf4223, Pallet created:2024-07-22</t>
+          <t>ID:fqnnrb6564, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ID:pyxban0787, Pallet created:2024-07-22</t>
+          <t>ID:shgrif5774, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ID:mflmdk3174, Pallet created:2024-07-22</t>
+          <t>ID:pkmbyn7847, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ID:rmngiw9286, Pallet created:2024-07-22</t>
+          <t>ID:funzwz3626, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ID:awxlfh6189, Pallet created:2024-07-22</t>
+          <t>ID:cnotkw1651, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ID:rtgxbi8232, Pallet created:2024-07-22</t>
+          <t>ID:jyxnrl1681, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ID:hukter9104, Pallet created:2024-07-22</t>
+          <t>ID:tykhsw4440, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ID:hfmxrq2002, Pallet created:2024-07-22</t>
+          <t>ID:vcchyj6440, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ID:ucjasj7633, Pallet created:2024-07-22</t>
+          <t>ID:uzhjgy7229, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ID:alsuvu0168, Pallet created:2024-07-22</t>
+          <t>ID:kibfcs9568, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ID:jzidjo4473, Pallet created:2024-07-22</t>
+          <t>ID:iqmvdv4163, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ID:xzpvcv2820, Pallet created:2024-07-22</t>
+          <t>ID:kywuaz1912, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ID:iwkjva1560, Pallet created:2024-07-22</t>
+          <t>ID:safygt0868, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ID:sfrxzf4201, Pallet created:2024-07-22</t>
+          <t>ID:oajlfz0692, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ID:chkebl9083, Pallet created:2024-07-22</t>
+          <t>ID:mlvich6792, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ID:tjquqs8665, Pallet created:2024-07-22</t>
+          <t>ID:ufvhxg6535, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ID:ygxtih3411, Pallet created:2024-07-22</t>
+          <t>ID:kycwyy9203, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ID:zgbymd0226, Pallet created:2024-07-22</t>
+          <t>ID:htnnwx2189, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ID:nfhopc1161, Pallet created:2024-07-22</t>
+          <t>ID:mqlyfb5328, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ID:ohgskv9278, Pallet created:2024-07-22</t>
+          <t>ID:vnoocg3138, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ID:azktmk2953, Pallet created:2024-07-22</t>
+          <t>ID:limogp5146, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ID:thfuga6618, Pallet created:2024-07-22</t>
+          <t>ID:pdwqax6605, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ID:vwnfcs5935, Pallet created:2024-07-22</t>
+          <t>ID:sngedu8286, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ID:hxpszh8267, Pallet created:2024-07-22</t>
+          <t>ID:bujkyg9280, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ID:dstsgm0902, Pallet created:2024-07-22</t>
+          <t>ID:kvnxtb4818, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ID:ahcavv0152, Pallet created:2024-07-22</t>
+          <t>ID:vcqndk9613, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ID:siguec4227, Pallet created:2024-07-22</t>
+          <t>ID:lpffhf0432, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ID:nrthoz1400, Pallet created:2024-07-22</t>
+          <t>ID:vtizbx2961, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ID:atgyvu4880, Pallet created:2024-07-22</t>
+          <t>ID:inbbfv0232, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ID:legiip6423, Pallet created:2024-07-22</t>
+          <t>ID:fvzlvr0677, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ID:rnuzhd7659, Pallet created:2024-07-22</t>
+          <t>ID:suabfc8773, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ID:nxrwbv4671, Pallet created:2024-07-22</t>
+          <t>ID:kttfkw1799, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ID:bvyygt0199, Pallet created:2024-07-22</t>
+          <t>ID:uluciy1365, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ID:odnkbg8998, Pallet created:2024-07-22</t>
+          <t>ID:ufifdz3281, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ID:mleaka9566, Pallet created:2024-07-22</t>
+          <t>ID:ryknxn5833, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ID:bujjci7325, Pallet created:2024-07-22</t>
+          <t>ID:ancbgx5749, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ID:myvrvh8965, Pallet created:2024-07-22</t>
+          <t>ID:yxzopc4050, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ID:fhgckd1575, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ID:qepetv3193, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ID:yooakf1109, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ID:swgkow7174, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ID:ivvnmu8221, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ID:jjytwz0225, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ID:qjzzdr4324, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ID:aatoet5944, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ID:pipqtv0661, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ID:nbupmd2535, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ID:yctxjp8403, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ID:tnprid7921, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ID:uyypqg2095, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ID:jzuzad7363, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ID:xgkcjc1291, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ID:mlsxcq9629, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ID:npixnp0584, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ID:cgzapm0489, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ID:tcmfap4496, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ID:ytoxtm1553, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ID:rvccxp7036, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ID:mpsplg6102, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ID:msgist5649, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ID:dpwcce9780, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ID:oxxdxh2054, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>ID:intowd0855, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ID:xpowle3734, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>ID:lvbvwv2078, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>ID:zxplvk4972, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>ID:gzpjbn0553, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>ID:wfiecc4774, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>ID:qdpkah0113, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>ID:myovgl2534, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>ID:oivpht1312, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ID:cejgpw9666, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>ID:aqznnz9290, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ID:pvdamm4293, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>ID:ulaucp6580, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ID:bqpydi7927, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ID:bwtotg8249, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ID:rmhbyt1866, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ID:xwsnri6759, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>ID:zgiosu9460, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>ID:jmaruj2342, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>ID:dfkyos8074, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>ID:hivouw8982, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>ID:akxyed5050, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ID:jncwbk3129, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ID:usykmw3570, Pallet created:2024-07-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>ID:olysyv6272, Pallet created:2024-07-23</t>
         </is>
       </c>
     </row>

</xml_diff>